<commit_message>
fixed one link and made the links clickable
</commit_message>
<xml_diff>
--- a/raw_data/alle_Anfragen_Beantwortungen/Parlamentsanfragen.xlsx
+++ b/raw_data/alle_Anfragen_Beantwortungen/Parlamentsanfragen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\WU\WARRA\raw_data\alle_Anfragen_Beantwortungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB89363E-0D66-4400-A2FC-F126CD1166E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E0C182-719B-4F53-AAED-FF1126B9200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6360" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Anfragen</t>
   </si>
@@ -253,16 +253,27 @@
   </si>
   <si>
     <t>https://www.parlament.gv.at/gegenstand/XXVII/AB/14381</t>
+  </si>
+  <si>
+    <t>https://www.parlament.gv.at/gegenstand/XXVII/J/7358</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -285,14 +296,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,7 +588,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,13 +640,13 @@
       <c r="C3" s="1">
         <v>45589</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F3" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>70</v>
       </c>
       <c r="H3" s="1">
@@ -649,13 +663,13 @@
       <c r="C4" s="1">
         <v>45495</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="1">
@@ -672,13 +686,13 @@
       <c r="C5" s="1">
         <v>45118</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="F5" t="s">
         <v>60</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H5" s="1">
@@ -695,13 +709,13 @@
       <c r="C6" s="1">
         <v>45110</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="1">
@@ -718,13 +732,13 @@
       <c r="C7" s="1">
         <v>44679</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="1">
@@ -741,13 +755,13 @@
       <c r="C8" s="1">
         <v>44386</v>
       </c>
-      <c r="D8" t="s">
-        <v>44</v>
+      <c r="D8" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H8" s="1">
@@ -764,13 +778,13 @@
       <c r="C9" s="1">
         <v>44294</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="H9" s="1">
@@ -787,13 +801,13 @@
       <c r="C10" s="1">
         <v>44018</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H10" s="1">
@@ -810,13 +824,13 @@
       <c r="C11" s="1">
         <v>43922</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>51</v>
       </c>
       <c r="H11" s="1">
@@ -833,13 +847,13 @@
       <c r="C12" s="1">
         <v>43888</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>54</v>
       </c>
       <c r="F12" t="s">
         <v>56</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>55</v>
       </c>
       <c r="H12" s="1">
@@ -856,13 +870,13 @@
       <c r="C14" s="1">
         <v>43402</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H14" s="1">
@@ -879,13 +893,13 @@
       <c r="C15" s="1">
         <v>42678</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="1">
@@ -902,13 +916,13 @@
       <c r="C18" s="1">
         <v>40234</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F18" t="s">
         <v>63</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="2" t="s">
         <v>62</v>
       </c>
       <c r="H18" s="1">
@@ -925,13 +939,13 @@
       <c r="C21" s="1">
         <v>45043</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F21" t="s">
         <v>71</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>75</v>
       </c>
       <c r="H21" s="1">
@@ -939,6 +953,36 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{09EBCD37-C762-4231-BB01-3D00C1D09661}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{1B083B35-817D-4B9C-94AF-B88D10733819}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{1A4C5C91-1578-45E8-8FB3-B0EE26224FCE}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{E9DA2118-9590-4050-B4F5-83B246C4365A}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{0A494E1F-D4C7-4A42-BA36-029C1AE06F5D}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{EE2AA8D6-EA44-4DED-8944-0EC716A1F9FB}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{53A76A29-4033-4C25-A2E8-DE41BACE18A1}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{17D9281A-D1A9-49EB-83C9-C8772D825C64}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{B71C50FC-9795-4A36-9FB3-27F07C8D501C}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{46B0B222-3394-4D79-AE81-EFE3D81606FA}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{60F08410-9266-4B02-A45B-A6ED6B8B9FDE}"/>
+    <hyperlink ref="D18" r:id="rId12" xr:uid="{CA889EAB-592F-4550-8482-12FE8BDE7136}"/>
+    <hyperlink ref="D21" r:id="rId13" xr:uid="{579C4D9A-F5E7-4A49-A8C4-C18D909C61CE}"/>
+    <hyperlink ref="G3" r:id="rId14" xr:uid="{BFA4AD67-84BE-4448-80D7-069C3D3B0D28}"/>
+    <hyperlink ref="G4" r:id="rId15" xr:uid="{D240AF28-6435-44C5-A148-47BD33B20B54}"/>
+    <hyperlink ref="G5" r:id="rId16" xr:uid="{BE719901-A31F-4437-B0E6-E9569087CF4A}"/>
+    <hyperlink ref="G6" r:id="rId17" xr:uid="{5591D575-BC50-48A0-8A13-F656A61BA2C7}"/>
+    <hyperlink ref="G7" r:id="rId18" xr:uid="{AECA2198-D741-4528-91D3-E003D5DEB8BB}"/>
+    <hyperlink ref="G8" r:id="rId19" xr:uid="{49457A95-55AE-4968-B462-8A54BB7C16DC}"/>
+    <hyperlink ref="G9" r:id="rId20" xr:uid="{356D08DC-B758-4F63-BD27-F33E5DA6CE8F}"/>
+    <hyperlink ref="G10" r:id="rId21" xr:uid="{E1F37126-9C38-4507-9D6E-D26AE484B7CB}"/>
+    <hyperlink ref="G11" r:id="rId22" xr:uid="{86F38C5D-1366-4E15-8976-D73B8E09922E}"/>
+    <hyperlink ref="G12" r:id="rId23" xr:uid="{E8E61A62-743E-47A2-93BF-69222ADE246E}"/>
+    <hyperlink ref="G14" r:id="rId24" xr:uid="{761DE619-AF9E-4E8F-9840-B3F63C72555B}"/>
+    <hyperlink ref="G15" r:id="rId25" xr:uid="{37DFA1F4-BF93-4DF7-8CA7-7A1F983A966C}"/>
+    <hyperlink ref="G18" r:id="rId26" xr:uid="{AF5C3B9A-9260-482E-A8D0-865C513F4325}"/>
+    <hyperlink ref="G21" r:id="rId27" xr:uid="{D334DE8F-94D0-4541-8B03-BD7B905245F2}"/>
+    <hyperlink ref="D12" r:id="rId28" xr:uid="{34E09D2D-FF92-476B-A63E-0FF3C463F089}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>